<commit_message>
Se actualizo el modelo de estimacion
</commit_message>
<xml_diff>
--- a/Modelo_de_Estimacion.xlsx
+++ b/Modelo_de_Estimacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de sistemas\Semestre 7\Ingenieria de software y requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de sistemas\Semestre 7\Ingenieria de software y requerimientos\Sistema_de_trasporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F3A6CD-A4FB-472D-B9D1-FCBFAE0BBCB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D026EE-F8B4-4B8A-8FBC-F9986710CC04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{62FADA92-7EC1-4AC9-9082-A929FFBB323A}"/>
   </bookViews>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1919CD18-48B0-4D53-ADD5-55E7744E5841}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,30 +1034,30 @@
         <v>27</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>119</v>
       </c>
       <c r="J2">
         <f>H2*F2</f>
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="K2">
         <f>J2/8</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L2" s="5">
         <f>VLOOKUP(G2,$P$2:$W$4,2,FALSE)*J2</f>
-        <v>294400</v>
+        <v>1177600</v>
       </c>
       <c r="M2" s="11">
         <f>J2/24</f>
-        <v>1.3333333333333333</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="N2" s="18">
         <f>(VLOOKUP(G2,$P$2:$W$4,2,FALSE)*(J2/3))+(VLOOKUP(G2,$P$2:$W$4,3,FALSE)*(J2/3))+(VLOOKUP(G2,$P$2:$W$4,5,FALSE)*(J2/3))</f>
-        <v>223932.89760348585</v>
+        <v>895731.5904139434</v>
       </c>
       <c r="P2" t="s">
         <v>27</v>
@@ -1106,30 +1106,30 @@
         <v>30</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
         <v>120</v>
       </c>
       <c r="J3">
         <f>H3*F3</f>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K47" si="0">J3/8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L3" s="5">
         <f>VLOOKUP(G3,$P$2:$W$4,2,FALSE)*J3</f>
-        <v>275472</v>
+        <v>550944</v>
       </c>
       <c r="M3" s="11">
         <f t="shared" ref="M3:M47" si="1">J3/24</f>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" ref="N3:N8" si="2">(VLOOKUP(G3,$P$2:$W$4,2,FALSE)*(J3/3))+(VLOOKUP(G3,$P$2:$W$4,3,FALSE)*(J3/3))+(VLOOKUP(G3,$P$2:$W$4,5,FALSE)*(J3/3))</f>
-        <v>203301.33333333331</v>
+        <v>406602.66666666663</v>
       </c>
       <c r="P3" t="s">
         <v>30</v>
@@ -1318,30 +1318,30 @@
         <v>30</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I6" t="s">
         <v>123</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="5"/>
-        <v>309906</v>
+        <v>619812</v>
       </c>
       <c r="M6" s="11">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="2"/>
-        <v>228714</v>
+        <v>457428</v>
       </c>
       <c r="P6" t="s">
         <v>36</v>
@@ -1389,30 +1389,30 @@
         <v>32</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
         <v>125</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="5"/>
-        <v>106155</v>
+        <v>212310</v>
       </c>
       <c r="M7" s="11">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="2"/>
-        <v>85013.529411764699</v>
+        <v>170027.0588235294</v>
       </c>
       <c r="Q7" t="s">
         <v>38</v>
@@ -1450,30 +1450,30 @@
         <v>32</v>
       </c>
       <c r="H8">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
         <v>126</v>
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="5"/>
-        <v>141540</v>
+        <v>283080</v>
       </c>
       <c r="M8" s="11">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="2"/>
-        <v>113351.37254901961</v>
+        <v>226702.74509803922</v>
       </c>
       <c r="P8" t="s">
         <v>42</v>
@@ -1514,30 +1514,30 @@
         <v>32</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
         <v>127</v>
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="5"/>
-        <v>141540</v>
+        <v>283080</v>
       </c>
       <c r="M9" s="11">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N9" s="5">
         <f>(VLOOKUP(G9,$P$2:$W$4,2,FALSE)*(J9/3))+(VLOOKUP(G9,$P$2:$W$4,3,FALSE)*(J9/3))+(VLOOKUP(G9,$P$2:$W$4,5,FALSE)*(J9/3))</f>
-        <v>113351.37254901961</v>
+        <v>226702.74509803922</v>
       </c>
       <c r="P9" t="s">
         <v>47</v>
@@ -1565,30 +1565,30 @@
         <v>30</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I10" t="s">
         <v>128</v>
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="5"/>
-        <v>103302</v>
+        <v>206604</v>
       </c>
       <c r="M10" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N10" s="5">
         <f t="shared" ref="N10:N47" si="8">(VLOOKUP(G10,$P$2:$W$4,2,FALSE)*(J10/3))+(VLOOKUP(G10,$P$2:$W$4,3,FALSE)*(J10/3))+(VLOOKUP(G10,$P$2:$W$4,5,FALSE)*(J10/3))</f>
-        <v>76238</v>
+        <v>152476</v>
       </c>
       <c r="P10" t="s">
         <v>52</v>
@@ -1609,30 +1609,30 @@
         <v>32</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I11" t="s">
         <v>129</v>
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="5"/>
-        <v>42462</v>
+        <v>84924</v>
       </c>
       <c r="M11" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N11" s="5">
         <f t="shared" si="8"/>
-        <v>34005.411764705881</v>
+        <v>68010.823529411762</v>
       </c>
       <c r="P11" t="s">
         <v>54</v>
@@ -1656,30 +1656,30 @@
         <v>32</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I12" t="s">
         <v>130</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="5"/>
-        <v>42462</v>
+        <v>84924</v>
       </c>
       <c r="M12" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" si="8"/>
-        <v>34005.411764705881</v>
+        <v>68010.823529411762</v>
       </c>
       <c r="P12" t="s">
         <v>57</v>
@@ -1700,30 +1700,30 @@
         <v>30</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I13" t="s">
         <v>123</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0.9375</v>
+        <v>1.875</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="5"/>
-        <v>129127.5</v>
+        <v>258255</v>
       </c>
       <c r="M13" s="11">
         <f t="shared" si="1"/>
-        <v>0.3125</v>
+        <v>0.625</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="8"/>
-        <v>95297.5</v>
+        <v>190595</v>
       </c>
       <c r="P13" t="s">
         <v>60</v>
@@ -1743,30 +1743,30 @@
         <v>30</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" t="s">
         <v>127</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>2.7</v>
+        <v>5.4</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>0.33750000000000002</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="5"/>
-        <v>46485.9</v>
+        <v>92971.8</v>
       </c>
       <c r="M14" s="11">
         <f t="shared" si="1"/>
-        <v>0.1125</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="8"/>
-        <v>34307.100000000006</v>
+        <v>68614.200000000012</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1783,30 +1783,30 @@
         <v>30</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
         <v>129</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="5"/>
-        <v>413208</v>
+        <v>826416</v>
       </c>
       <c r="M15" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="8"/>
-        <v>304952</v>
+        <v>609904</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
@@ -1823,30 +1823,30 @@
         <v>30</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I16" t="s">
         <v>120</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="5"/>
-        <v>275472</v>
+        <v>550944</v>
       </c>
       <c r="M16" s="11">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="8"/>
-        <v>203301.33333333331</v>
+        <v>406602.66666666663</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
@@ -1863,30 +1863,30 @@
         <v>30</v>
       </c>
       <c r="H17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I17" t="s">
         <v>126</v>
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>3.125</v>
+        <v>6.25</v>
       </c>
       <c r="L17" s="5">
         <f t="shared" si="5"/>
-        <v>430425</v>
+        <v>860850</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" si="1"/>
-        <v>1.0416666666666667</v>
+        <v>2.0833333333333335</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="8"/>
-        <v>317658.33333333337</v>
+        <v>635316.66666666674</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
@@ -1903,30 +1903,30 @@
         <v>30</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" t="s">
         <v>129</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" s="5">
         <f t="shared" si="5"/>
-        <v>137736</v>
+        <v>275472</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="8"/>
-        <v>101650.66666666666</v>
+        <v>203301.33333333331</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
@@ -1943,30 +1943,30 @@
         <v>30</v>
       </c>
       <c r="H19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I19" t="s">
         <v>126</v>
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="5"/>
-        <v>826416</v>
+        <v>1652832</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="8"/>
-        <v>609904</v>
+        <v>1219808</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
@@ -1983,30 +1983,30 @@
         <v>30</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I20" t="s">
         <v>131</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L20" s="5">
         <f t="shared" si="5"/>
-        <v>275472</v>
+        <v>550944</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="8"/>
-        <v>203301.33333333331</v>
+        <v>406602.66666666663</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
@@ -2029,30 +2029,30 @@
         <v>32</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I21" t="s">
         <v>132</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" si="5"/>
-        <v>679392</v>
+        <v>1358784</v>
       </c>
       <c r="M21" s="11">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="8"/>
-        <v>544086.5882352941</v>
+        <v>1088173.1764705882</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
@@ -2069,30 +2069,30 @@
         <v>32</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
         <v>133</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>0.4375</v>
+        <v>0.875</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="5"/>
-        <v>24769.5</v>
+        <v>49539</v>
       </c>
       <c r="M22" s="11">
         <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="8"/>
-        <v>19836.490196078434</v>
+        <v>39672.980392156867</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
@@ -2109,30 +2109,30 @@
         <v>32</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I23" t="s">
         <v>134</v>
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="5"/>
-        <v>141540</v>
+        <v>283080</v>
       </c>
       <c r="M23" s="11">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="8"/>
-        <v>113351.37254901961</v>
+        <v>226702.74509803922</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
@@ -2149,30 +2149,30 @@
         <v>30</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
         <v>135</v>
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="5"/>
-        <v>68868</v>
+        <v>137736</v>
       </c>
       <c r="M24" s="11">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="8"/>
-        <v>50825.333333333328</v>
+        <v>101650.66666666666</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
@@ -2189,30 +2189,30 @@
         <v>30</v>
       </c>
       <c r="H25">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I25" t="s">
         <v>129</v>
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="5"/>
-        <v>258255</v>
+        <v>516510</v>
       </c>
       <c r="M25" s="11">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="8"/>
-        <v>190595</v>
+        <v>381190</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
@@ -2229,30 +2229,30 @@
         <v>32</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
         <v>121</v>
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>2.8125</v>
+        <v>5.625</v>
       </c>
       <c r="L26" s="5">
         <f t="shared" si="5"/>
-        <v>159232.5</v>
+        <v>318465</v>
       </c>
       <c r="M26" s="11">
         <f t="shared" si="1"/>
-        <v>0.9375</v>
+        <v>1.875</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="8"/>
-        <v>127520.29411764705</v>
+        <v>255040.5882352941</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
@@ -2269,30 +2269,30 @@
         <v>32</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I27" t="s">
         <v>126</v>
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="L27" s="5">
         <f t="shared" si="5"/>
-        <v>70770</v>
+        <v>141540</v>
       </c>
       <c r="M27" s="11">
         <f t="shared" si="1"/>
-        <v>0.41666666666666669</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="8"/>
-        <v>56675.686274509804</v>
+        <v>113351.37254901961</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
@@ -2315,30 +2315,30 @@
         <v>30</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
         <v>128</v>
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L28" s="5">
         <f t="shared" si="5"/>
-        <v>688680</v>
+        <v>1377360</v>
       </c>
       <c r="M28" s="11">
         <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="8"/>
-        <v>508253.33333333337</v>
+        <v>1016506.6666666667</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
@@ -2355,30 +2355,30 @@
         <v>32</v>
       </c>
       <c r="H29">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="I29" t="s">
         <v>132</v>
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>1.875</v>
+        <v>3.75</v>
       </c>
       <c r="L29" s="5">
         <f t="shared" si="5"/>
-        <v>106155</v>
+        <v>212310</v>
       </c>
       <c r="M29" s="11">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="8"/>
-        <v>85013.529411764699</v>
+        <v>170027.0588235294</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
@@ -2395,30 +2395,30 @@
         <v>32</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I30" t="s">
         <v>120</v>
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="5"/>
-        <v>28308</v>
+        <v>56616</v>
       </c>
       <c r="M30" s="11">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="8"/>
-        <v>22670.274509803919</v>
+        <v>45340.549019607839</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
@@ -2435,30 +2435,30 @@
         <v>30</v>
       </c>
       <c r="H31">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="L31" s="5">
         <f t="shared" si="5"/>
-        <v>619812</v>
+        <v>1239624</v>
       </c>
       <c r="M31" s="11">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="8"/>
-        <v>457428</v>
+        <v>914856</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
@@ -2475,30 +2475,30 @@
         <v>32</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I32" t="s">
         <v>137</v>
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L32" s="5">
         <f t="shared" si="5"/>
-        <v>56616</v>
+        <v>113232</v>
       </c>
       <c r="M32" s="11">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="8"/>
-        <v>45340.549019607839</v>
+        <v>90681.098039215678</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -2515,30 +2515,30 @@
         <v>30</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I33" t="s">
         <v>138</v>
       </c>
       <c r="J33">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="L33" s="5">
         <f t="shared" si="5"/>
-        <v>206604</v>
+        <v>413208</v>
       </c>
       <c r="M33" s="11">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="8"/>
-        <v>152476</v>
+        <v>304952</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -2561,30 +2561,30 @@
         <v>30</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34" t="s">
         <v>139</v>
       </c>
       <c r="J34">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="L34" s="5">
         <f t="shared" si="5"/>
-        <v>103302</v>
+        <v>206604</v>
       </c>
       <c r="M34" s="11">
         <f t="shared" si="1"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="8"/>
-        <v>76238</v>
+        <v>152476</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -2601,30 +2601,30 @@
         <v>30</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35" t="s">
         <v>140</v>
       </c>
       <c r="J35">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>1.25</v>
       </c>
       <c r="L35" s="5">
         <f t="shared" si="5"/>
-        <v>86085</v>
+        <v>172170</v>
       </c>
       <c r="M35" s="11">
         <f t="shared" si="1"/>
-        <v>0.20833333333333334</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="8"/>
-        <v>63531.666666666672</v>
+        <v>127063.33333333334</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2641,30 +2641,30 @@
         <v>30</v>
       </c>
       <c r="H36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I36" t="s">
         <v>141</v>
       </c>
       <c r="J36">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K36">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="L36" s="5">
         <f t="shared" si="5"/>
-        <v>206604</v>
+        <v>413208</v>
       </c>
       <c r="M36" s="11">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="8"/>
-        <v>152476</v>
+        <v>304952</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -2681,30 +2681,30 @@
         <v>30</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I37" t="s">
         <v>126</v>
       </c>
       <c r="J37">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K37">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L37" s="5">
         <f t="shared" si="5"/>
-        <v>137736</v>
+        <v>275472</v>
       </c>
       <c r="M37" s="11">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N37" s="5">
         <f t="shared" si="8"/>
-        <v>101650.66666666666</v>
+        <v>203301.33333333331</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -2721,30 +2721,30 @@
         <v>30</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
         <v>132</v>
       </c>
       <c r="J38">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" si="5"/>
-        <v>206604</v>
+        <v>413208</v>
       </c>
       <c r="M38" s="11">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N38" s="5">
         <f t="shared" si="8"/>
-        <v>152476</v>
+        <v>304952</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -2767,30 +2767,30 @@
         <v>30</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I39" t="s">
         <v>129</v>
       </c>
       <c r="J39">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L39" s="5">
         <f t="shared" si="5"/>
-        <v>413208</v>
+        <v>826416</v>
       </c>
       <c r="M39" s="11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N39" s="5">
         <f t="shared" si="8"/>
-        <v>304952</v>
+        <v>609904</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -2807,30 +2807,30 @@
         <v>30</v>
       </c>
       <c r="H40">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I40" t="s">
         <v>128</v>
       </c>
       <c r="J40">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K40">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L40" s="5">
         <f t="shared" si="5"/>
-        <v>275472</v>
+        <v>550944</v>
       </c>
       <c r="M40" s="11">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N40" s="5">
         <f t="shared" si="8"/>
-        <v>203301.33333333331</v>
+        <v>406602.66666666663</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
@@ -2847,30 +2847,30 @@
         <v>30</v>
       </c>
       <c r="H41">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I41" t="s">
         <v>120</v>
       </c>
       <c r="J41">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K41">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L41" s="5">
         <f t="shared" si="5"/>
-        <v>344340</v>
+        <v>688680</v>
       </c>
       <c r="M41" s="11">
         <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="N41" s="5">
         <f t="shared" si="8"/>
-        <v>254126.66666666669</v>
+        <v>508253.33333333337</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
@@ -2887,30 +2887,30 @@
         <v>30</v>
       </c>
       <c r="H42">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I42" t="s">
         <v>138</v>
       </c>
       <c r="J42">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K42">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="L42" s="5">
         <f t="shared" si="5"/>
-        <v>206604</v>
+        <v>413208</v>
       </c>
       <c r="M42" s="11">
         <f>J42/24</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N42" s="5">
         <f t="shared" si="8"/>
-        <v>152476</v>
+        <v>304952</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -2933,30 +2933,30 @@
         <v>30</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
         <v>122</v>
       </c>
       <c r="J43">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="K43">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L43" s="5">
         <f t="shared" si="5"/>
-        <v>275472</v>
+        <v>550944</v>
       </c>
       <c r="M43" s="11">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="N43" s="5">
         <f t="shared" si="8"/>
-        <v>203301.33333333331</v>
+        <v>406602.66666666663</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -2973,30 +2973,30 @@
         <v>30</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I44" t="s">
         <v>123</v>
       </c>
       <c r="J44">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="K44">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L44" s="5">
         <f t="shared" si="5"/>
-        <v>550944</v>
+        <v>1101888</v>
       </c>
       <c r="M44" s="11">
         <f t="shared" si="1"/>
-        <v>1.3333333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="N44" s="5">
         <f t="shared" si="8"/>
-        <v>406602.66666666663</v>
+        <v>813205.33333333326</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -3013,30 +3013,30 @@
         <v>30</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
         <v>142</v>
       </c>
       <c r="J45">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L45" s="5">
         <f t="shared" si="5"/>
-        <v>137736</v>
+        <v>275472</v>
       </c>
       <c r="M45" s="11">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="N45" s="5">
         <f t="shared" si="8"/>
-        <v>101650.66666666666</v>
+        <v>203301.33333333331</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -3053,30 +3053,30 @@
         <v>30</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I46" t="s">
         <v>143</v>
       </c>
       <c r="J46">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K46">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L46" s="5">
         <f t="shared" si="5"/>
-        <v>1101888</v>
+        <v>2203776</v>
       </c>
       <c r="M46" s="11">
         <f t="shared" si="1"/>
-        <v>2.6666666666666665</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="N46" s="5">
         <f t="shared" si="8"/>
-        <v>813205.33333333326</v>
+        <v>1626410.6666666665</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -3096,30 +3096,30 @@
         <v>30</v>
       </c>
       <c r="H47" s="13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I47" s="13" t="s">
         <v>144</v>
       </c>
       <c r="J47" s="13">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>320</v>
       </c>
       <c r="K47" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="L47" s="15">
         <f t="shared" si="5"/>
-        <v>2754720</v>
+        <v>5509440</v>
       </c>
       <c r="M47" s="16">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="N47" s="15">
         <f t="shared" si="8"/>
-        <v>2033013.3333333335</v>
+        <v>4066026.666666667</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -3128,11 +3128,11 @@
       </c>
       <c r="L48" s="17">
         <f>SUM(L2:L47)</f>
-        <v>15054837.4</v>
+        <v>29544935.800000001</v>
       </c>
       <c r="N48" s="17">
         <f>SUM(N2:N47)</f>
-        <v>11226684.046623096</v>
+        <v>22049909.555119827</v>
       </c>
     </row>
     <row r="49" spans="11:14" x14ac:dyDescent="0.3">
@@ -3141,17 +3141,17 @@
       </c>
       <c r="L49" s="9">
         <f>L48*1.68</f>
-        <v>25292126.831999999</v>
+        <v>49635492.144000001</v>
       </c>
       <c r="N49" s="9">
-        <f>L48-N48</f>
-        <v>3828153.3533769045</v>
+        <f>N48*1.68</f>
+        <v>37043848.052601308</v>
       </c>
     </row>
     <row r="50" spans="11:14" x14ac:dyDescent="0.3">
       <c r="N50" s="9">
-        <f>N49*1.68</f>
-        <v>6431297.6336731995</v>
+        <f>L48-N48</f>
+        <v>7495026.2448801734</v>
       </c>
     </row>
     <row r="51" spans="11:14" x14ac:dyDescent="0.3">

</xml_diff>